<commit_message>
Added feed back to audio amp / change audio CC cap Reviewd - this looks good for release
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for TechDemo/REV2/Generate Files/BOM/Bill of Materials-TechDemo(Normal Build Variant of TechDemo).xlsx
+++ b/Hardware/Project Outputs for TechDemo/REV2/Generate Files/BOM/Bill of Materials-TechDemo(Normal Build Variant of TechDemo).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="534">
   <si>
     <t xml:space="preserve">Column=LibRef</t>
   </si>
@@ -222,13 +222,13 @@
     <t xml:space="preserve">H. Collector</t>
   </si>
   <si>
-    <t xml:space="preserve">4/16/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:31 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">233</t>
+    <t xml:space="preserve">4/17/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:39 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity</t>
@@ -258,6 +258,9 @@
     <t xml:space="preserve">CAP_22UF_10V_TANT</t>
   </si>
   <si>
+    <t xml:space="preserve">CAP_10UF_50V_1206</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAP_1.0UF_50V_0805</t>
   </si>
   <si>
@@ -273,9 +276,6 @@
     <t xml:space="preserve">CAP_18NF_50V_0805</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP_10UF_50V_1206</t>
-  </si>
-  <si>
     <t xml:space="preserve">DIODE_1N4148W-7-F</t>
   </si>
   <si>
@@ -294,9 +294,6 @@
     <t xml:space="preserve">FERRITE_BLM21AG102SN1D</t>
   </si>
   <si>
-    <t xml:space="preserve">CONN_6P_SINGLE_ROW</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONN_HIROSE_DM3BT-DSF-PEJS</t>
   </si>
   <si>
@@ -486,6 +483,9 @@
     <t xml:space="preserve">CAP TANT 22UF 20% 10V 1206</t>
   </si>
   <si>
+    <t xml:space="preserve">CAP CER 10UF 50V X5R 1206</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAP CER 1UF 50V X7R 0805</t>
   </si>
   <si>
@@ -501,9 +501,6 @@
     <t xml:space="preserve">CAP CER 0.018UF 50V X7R 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP CER 10UF 50V X5R 1206</t>
-  </si>
-  <si>
     <t xml:space="preserve">DIODE GEN PURP 100V 300MA SOD123</t>
   </si>
   <si>
@@ -522,9 +519,6 @@
     <t xml:space="preserve">FERRITE, 1KOHM AT 100MHZ, 220MA, .450DCR</t>
   </si>
   <si>
-    <t xml:space="preserve">CONN HEADER VERT 6POS 2.54MM</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONN MICRO SD CARD PUSH-PUSH R/A</t>
   </si>
   <si>
@@ -693,7 +687,7 @@
     <t xml:space="preserve">BAT1</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C22, C23, C24, C25, C26, C27, C28, C29, C54, C61, C62, C63, C74</t>
+    <t xml:space="preserve">C1, C22, C23, C24, C25, C26, C27, C28, C29, C61, C62, C63, C74</t>
   </si>
   <si>
     <t xml:space="preserve">C4, C5</t>
@@ -711,6 +705,9 @@
     <t xml:space="preserve">C46, C49, C77, C78</t>
   </si>
   <si>
+    <t xml:space="preserve">C54, C84, C85</t>
+  </si>
+  <si>
     <t xml:space="preserve">C55</t>
   </si>
   <si>
@@ -726,9 +723,6 @@
     <t xml:space="preserve">C73</t>
   </si>
   <si>
-    <t xml:space="preserve">C84, C85</t>
-  </si>
-  <si>
     <t xml:space="preserve">D1, D5, D6, D8, D10</t>
   </si>
   <si>
@@ -747,9 +741,6 @@
     <t xml:space="preserve">FB1, FB2, FB3, FB4, FB5</t>
   </si>
   <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
     <t xml:space="preserve">J3</t>
   </si>
   <si>
@@ -960,15 +951,15 @@
     <t xml:space="preserve">MURATA</t>
   </si>
   <si>
+    <t xml:space="preserve">Hirose Electric Co Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sullins Connector Solutions</t>
   </si>
   <si>
-    <t xml:space="preserve">Hirose Electric Co Ltd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molex</t>
-  </si>
-  <si>
     <t xml:space="preserve">COILCRAFT</t>
   </si>
   <si>
@@ -1050,6 +1041,9 @@
     <t xml:space="preserve">TAJA226M010RNJ</t>
   </si>
   <si>
+    <t xml:space="preserve">CL31A106KBHNNNE</t>
+  </si>
+  <si>
     <t xml:space="preserve">UMK212B7105MGHT</t>
   </si>
   <si>
@@ -1065,9 +1059,6 @@
     <t xml:space="preserve">CC0805KRX7R9BB183</t>
   </si>
   <si>
-    <t xml:space="preserve">CL31A106KBHNNNE</t>
-  </si>
-  <si>
     <t xml:space="preserve">1N4148W-7-F</t>
   </si>
   <si>
@@ -1086,9 +1077,6 @@
     <t xml:space="preserve">BLM21AG102SN1D</t>
   </si>
   <si>
-    <t xml:space="preserve">PREC006SFAN-RC</t>
-  </si>
-  <si>
     <t xml:space="preserve">DM3BT-DSF-PEJS</t>
   </si>
   <si>
@@ -1290,6 +1278,9 @@
     <t xml:space="preserve">478-5798-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">1276-2876-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">587-6375-1-ND</t>
   </si>
   <si>
@@ -1305,9 +1296,6 @@
     <t xml:space="preserve">311-1137-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">1276-2876-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">1N4148W-FDICT-ND</t>
   </si>
   <si>
@@ -1323,9 +1311,6 @@
     <t xml:space="preserve">490-1041-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">S1212EC-06-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">HR1942CT-ND</t>
   </si>
   <si>
@@ -1503,12 +1488,12 @@
     <t xml:space="preserve">CAP_1206_TANT</t>
   </si>
   <si>
+    <t xml:space="preserve">CAP_1206</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAP_2312</t>
   </si>
   <si>
-    <t xml:space="preserve">CAP_1206</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOD123</t>
   </si>
   <si>
@@ -1524,9 +1509,6 @@
     <t xml:space="preserve">RES_0805</t>
   </si>
   <si>
-    <t xml:space="preserve">HDR_1X6_100MILL</t>
-  </si>
-  <si>
     <t xml:space="preserve">HRS_DM3BT-DSF-PEJS</t>
   </si>
   <si>
@@ -1629,7 +1611,7 @@
     <t xml:space="preserve">Bill of Materials for Variant [Normal Build Variant of TechDemo] of Project [TechDemo.PrjPcb] (No PCB Document Selected)</t>
   </si>
   <si>
-    <t xml:space="preserve">4/16/2021 10:31 AM</t>
+    <t xml:space="preserve">4/17/2021 1:39 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Bill of Materials</t>
@@ -3029,11 +3011,11 @@
       </c>
       <c r="E8" s="41">
         <f ca="1">TODAY()</f>
-        <v>44302</v>
+        <v>44303</v>
       </c>
       <c r="F8" s="42">
         <f ca="1">NOW()</f>
-        <v>44302.4386936151</v>
+        <v>44303.5688027056</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="39"/>
@@ -3055,25 +3037,25 @@
         <v>69</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="I9" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="J9" s="26" t="s">
         <v>409</v>
       </c>
-      <c r="J9" s="26" t="s">
-        <v>413</v>
-      </c>
       <c r="K9" s="27" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -3092,22 +3074,22 @@
         <v>70</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G10" s="62" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H10" s="62" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I10" s="62" t="s">
+        <v>406</v>
+      </c>
+      <c r="J10" s="62" t="s">
         <v>410</v>
-      </c>
-      <c r="J10" s="62" t="s">
-        <v>414</v>
       </c>
       <c r="K10" s="54" t="s">
         <v>70</v>
@@ -3122,31 +3104,31 @@
         <v>2</v>
       </c>
       <c r="C11" s="65">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>71</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G11" s="60" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H11" s="60" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I11" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J11" s="60" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="K11" s="55" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -3164,25 +3146,25 @@
         <v>72</v>
       </c>
       <c r="E12" s="59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G12" s="62" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H12" s="62" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="I12" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J12" s="62" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="K12" s="54" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -3200,25 +3182,25 @@
         <v>73</v>
       </c>
       <c r="E13" s="60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G13" s="60" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H13" s="60" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I13" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J13" s="60" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="K13" s="55" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -3236,25 +3218,25 @@
         <v>74</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F14" s="62" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G14" s="62" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H14" s="62" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I14" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J14" s="62" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="K14" s="54" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -3272,25 +3254,25 @@
         <v>75</v>
       </c>
       <c r="E15" s="60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15" s="60" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G15" s="60" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H15" s="60" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="I15" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J15" s="60" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="K15" s="55" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="L15"/>
       <c r="M15"/>
@@ -3308,25 +3290,25 @@
         <v>76</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F16" s="62" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G16" s="62" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H16" s="62" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I16" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="K16" s="54" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="L16"/>
       <c r="M16"/>
@@ -3338,31 +3320,31 @@
         <v>8</v>
       </c>
       <c r="C17" s="65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" s="60" t="s">
         <v>77</v>
       </c>
       <c r="E17" s="60" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G17" s="60" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="H17" s="60" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="I17" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J17" s="60" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="K17" s="55" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="L17"/>
       <c r="M17"/>
@@ -3374,31 +3356,31 @@
         <v>9</v>
       </c>
       <c r="C18" s="64">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="59" t="s">
         <v>78</v>
       </c>
       <c r="E18" s="59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G18" s="62" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="H18" s="62" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J18" s="62" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="K18" s="54" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="L18"/>
       <c r="M18"/>
@@ -3410,31 +3392,31 @@
         <v>10</v>
       </c>
       <c r="C19" s="65">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D19" s="60" t="s">
         <v>79</v>
       </c>
       <c r="E19" s="60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F19" s="60" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G19" s="60" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H19" s="60" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I19" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J19" s="60" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="K19" s="55" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L19"/>
       <c r="M19"/>
@@ -3446,31 +3428,31 @@
         <v>11</v>
       </c>
       <c r="C20" s="64">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D20" s="59" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F20" s="62" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G20" s="62" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H20" s="62" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="I20" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J20" s="62" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="K20" s="54" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="L20"/>
       <c r="M20"/>
@@ -3488,25 +3470,25 @@
         <v>81</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F21" s="60" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G21" s="60" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H21" s="60" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I21" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J21" s="60" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="K21" s="55" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="L21"/>
       <c r="M21"/>
@@ -3518,31 +3500,31 @@
         <v>13</v>
       </c>
       <c r="C22" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="59" t="s">
         <v>82</v>
       </c>
       <c r="E22" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F22" s="62" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G22" s="62" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="H22" s="62" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I22" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J22" s="62" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="K22" s="54" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="L22"/>
       <c r="M22"/>
@@ -3560,25 +3542,25 @@
         <v>83</v>
       </c>
       <c r="E23" s="60" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F23" s="60" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G23" s="60" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H23" s="60" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I23" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J23" s="60" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="K23" s="55" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="L23"/>
       <c r="M23"/>
@@ -3596,25 +3578,25 @@
         <v>84</v>
       </c>
       <c r="E24" s="59" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F24" s="62" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G24" s="62" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H24" s="62" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I24" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="K24" s="54" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="L24"/>
       <c r="M24"/>
@@ -3632,25 +3614,25 @@
         <v>85</v>
       </c>
       <c r="E25" s="60" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F25" s="60" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G25" s="60" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H25" s="60" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I25" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J25" s="60" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="K25" s="55" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="L25"/>
       <c r="M25"/>
@@ -3668,25 +3650,25 @@
         <v>86</v>
       </c>
       <c r="E26" s="59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F26" s="62" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G26" s="62" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H26" s="62" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I26" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="K26" s="54" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="L26"/>
       <c r="M26"/>
@@ -3704,25 +3686,25 @@
         <v>87</v>
       </c>
       <c r="E27" s="60" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F27" s="60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G27" s="60" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H27" s="60" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I27" s="60" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="J27" s="60" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="K27" s="55" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="L27"/>
       <c r="M27"/>
@@ -3740,25 +3722,25 @@
         <v>88</v>
       </c>
       <c r="E28" s="59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F28" s="62" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G28" s="62" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H28" s="62" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="I28" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J28" s="62" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="L28"/>
       <c r="M28"/>
@@ -3776,25 +3758,25 @@
         <v>89</v>
       </c>
       <c r="E29" s="60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F29" s="60" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G29" s="60" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H29" s="60" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I29" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J29" s="60" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="K29" s="55" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="L29"/>
       <c r="M29"/>
@@ -3812,25 +3794,25 @@
         <v>90</v>
       </c>
       <c r="E30" s="59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F30" s="62" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G30" s="62" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H30" s="62" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I30" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J30" s="62" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="K30" s="54" t="s">
-        <v>500</v>
+        <v>90</v>
       </c>
       <c r="L30"/>
       <c r="M30"/>
@@ -3848,22 +3830,22 @@
         <v>91</v>
       </c>
       <c r="E31" s="60" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F31" s="60" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G31" s="60" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="H31" s="60" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="I31" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J31" s="60" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K31" s="55" t="s">
         <v>91</v>
@@ -3884,25 +3866,25 @@
         <v>92</v>
       </c>
       <c r="E32" s="59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F32" s="62" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G32" s="62" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="H32" s="62" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I32" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J32" s="62" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="K32" s="54" t="s">
-        <v>92</v>
+        <v>495</v>
       </c>
       <c r="L32"/>
       <c r="M32"/>
@@ -3914,31 +3896,31 @@
         <v>24</v>
       </c>
       <c r="C33" s="65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="60" t="s">
         <v>93</v>
       </c>
       <c r="E33" s="60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F33" s="60" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G33" s="60" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H33" s="60" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="I33" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J33" s="60" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="K33" s="55" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="L33"/>
       <c r="M33"/>
@@ -3950,31 +3932,31 @@
         <v>25</v>
       </c>
       <c r="C34" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="59" t="s">
         <v>94</v>
       </c>
       <c r="E34" s="59" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F34" s="62" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G34" s="62" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H34" s="62" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="I34" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J34" s="62" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="K34" s="54" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="L34"/>
       <c r="M34"/>
@@ -3992,25 +3974,25 @@
         <v>95</v>
       </c>
       <c r="E35" s="60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F35" s="60" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G35" s="60" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H35" s="60" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="I35" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J35" s="60" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="K35" s="55" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="L35"/>
       <c r="M35"/>
@@ -4028,25 +4010,25 @@
         <v>96</v>
       </c>
       <c r="E36" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F36" s="62" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G36" s="62" t="s">
         <v>311</v>
       </c>
       <c r="H36" s="62" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="I36" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J36" s="62" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="K36" s="54" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="L36"/>
       <c r="M36"/>
@@ -4064,25 +4046,25 @@
         <v>97</v>
       </c>
       <c r="E37" s="60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F37" s="60" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G37" s="60" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H37" s="60" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I37" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J37" s="60" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="K37" s="55" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="L37"/>
       <c r="M37"/>
@@ -4100,25 +4082,25 @@
         <v>98</v>
       </c>
       <c r="E38" s="59" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F38" s="62" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G38" s="62" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H38" s="62" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="I38" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J38" s="62" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="K38" s="54" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="L38"/>
       <c r="M38"/>
@@ -4136,25 +4118,25 @@
         <v>99</v>
       </c>
       <c r="E39" s="60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F39" s="60" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G39" s="60" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H39" s="60" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I39" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J39" s="60" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="K39" s="55" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="L39"/>
       <c r="M39"/>
@@ -4172,25 +4154,25 @@
         <v>100</v>
       </c>
       <c r="E40" s="59" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F40" s="62" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G40" s="62" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H40" s="62" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="I40" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J40" s="62" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="K40" s="54" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="L40"/>
       <c r="M40"/>
@@ -4202,31 +4184,31 @@
         <v>32</v>
       </c>
       <c r="C41" s="65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D41" s="60" t="s">
         <v>101</v>
       </c>
       <c r="E41" s="60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F41" s="60" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G41" s="60" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H41" s="60" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I41" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J41" s="60" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K41" s="55" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="L41"/>
       <c r="M41"/>
@@ -4244,25 +4226,25 @@
         <v>102</v>
       </c>
       <c r="E42" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F42" s="62" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G42" s="62" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="H42" s="62" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="I42" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J42" s="62" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="K42" s="54" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="L42"/>
       <c r="M42"/>
@@ -4274,31 +4256,31 @@
         <v>34</v>
       </c>
       <c r="C43" s="65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D43" s="60" t="s">
         <v>103</v>
       </c>
       <c r="E43" s="60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F43" s="60" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G43" s="60" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="H43" s="60" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="I43" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J43" s="60" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="K43" s="55" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="L43"/>
       <c r="M43"/>
@@ -4316,25 +4298,25 @@
         <v>104</v>
       </c>
       <c r="E44" s="59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F44" s="62" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G44" s="62" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H44" s="62" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="I44" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J44" s="62" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="K44" s="54" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="L44"/>
       <c r="M44"/>
@@ -4346,31 +4328,31 @@
         <v>36</v>
       </c>
       <c r="C45" s="65">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D45" s="60" t="s">
         <v>105</v>
       </c>
       <c r="E45" s="60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F45" s="60" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G45" s="60" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H45" s="60" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I45" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J45" s="60" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="K45" s="55" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="L45"/>
       <c r="M45"/>
@@ -4382,31 +4364,31 @@
         <v>37</v>
       </c>
       <c r="C46" s="64">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D46" s="59" t="s">
         <v>106</v>
       </c>
       <c r="E46" s="59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F46" s="62" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G46" s="62" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H46" s="62" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="I46" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J46" s="62" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="K46" s="54" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="L46"/>
       <c r="M46"/>
@@ -4418,31 +4400,31 @@
         <v>38</v>
       </c>
       <c r="C47" s="65">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D47" s="60" t="s">
         <v>107</v>
       </c>
       <c r="E47" s="60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F47" s="60" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G47" s="60" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="H47" s="60" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="I47" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J47" s="60" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="K47" s="55" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="L47"/>
       <c r="M47"/>
@@ -4454,31 +4436,31 @@
         <v>39</v>
       </c>
       <c r="C48" s="64">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D48" s="59" t="s">
         <v>108</v>
       </c>
       <c r="E48" s="59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F48" s="62" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G48" s="62" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H48" s="62" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I48" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J48" s="62" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="K48" s="54" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="L48"/>
       <c r="M48"/>
@@ -4490,31 +4472,31 @@
         <v>40</v>
       </c>
       <c r="C49" s="65">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D49" s="60" t="s">
         <v>109</v>
       </c>
       <c r="E49" s="60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F49" s="60" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G49" s="60" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="H49" s="60" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I49" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J49" s="60" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="K49" s="55" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="L49"/>
       <c r="M49"/>
@@ -4526,31 +4508,31 @@
         <v>41</v>
       </c>
       <c r="C50" s="64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="59" t="s">
         <v>110</v>
       </c>
       <c r="E50" s="59" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F50" s="62" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G50" s="62" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H50" s="62" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="I50" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J50" s="62" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="K50" s="54" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="L50"/>
       <c r="M50"/>
@@ -4568,25 +4550,25 @@
         <v>111</v>
       </c>
       <c r="E51" s="60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F51" s="60" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G51" s="60" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="H51" s="60" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I51" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J51" s="60" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="K51" s="55" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="L51"/>
       <c r="M51"/>
@@ -4598,31 +4580,31 @@
         <v>43</v>
       </c>
       <c r="C52" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" s="59" t="s">
         <v>112</v>
       </c>
       <c r="E52" s="59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F52" s="62" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G52" s="62" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="H52" s="62" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="I52" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J52" s="62" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="K52" s="54" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="L52"/>
       <c r="M52"/>
@@ -4640,25 +4622,25 @@
         <v>113</v>
       </c>
       <c r="E53" s="60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F53" s="60" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G53" s="60" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="H53" s="60" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I53" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J53" s="60" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="K53" s="55" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
       <c r="L53"/>
       <c r="M53"/>
@@ -4676,25 +4658,25 @@
         <v>114</v>
       </c>
       <c r="E54" s="59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F54" s="62" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G54" s="62" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H54" s="62" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="I54" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J54" s="62" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="K54" s="54" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
       <c r="L54"/>
       <c r="M54"/>
@@ -4712,25 +4694,25 @@
         <v>115</v>
       </c>
       <c r="E55" s="60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F55" s="60" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G55" s="60" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H55" s="60" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I55" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J55" s="60" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="K55" s="55" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="L55"/>
       <c r="M55"/>
@@ -4748,25 +4730,25 @@
         <v>116</v>
       </c>
       <c r="E56" s="59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F56" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G56" s="62" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H56" s="62" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I56" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J56" s="62" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="K56" s="54" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="L56"/>
       <c r="M56"/>
@@ -4784,25 +4766,25 @@
         <v>117</v>
       </c>
       <c r="E57" s="60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F57" s="60" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G57" s="60" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H57" s="60" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I57" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J57" s="60" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="K57" s="55" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="L57"/>
       <c r="M57"/>
@@ -4820,25 +4802,25 @@
         <v>118</v>
       </c>
       <c r="E58" s="59" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F58" s="62" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G58" s="62" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H58" s="62" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I58" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J58" s="62" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="K58" s="54" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="L58"/>
       <c r="M58"/>
@@ -4850,31 +4832,31 @@
         <v>50</v>
       </c>
       <c r="C59" s="65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59" s="60" t="s">
         <v>119</v>
       </c>
       <c r="E59" s="60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F59" s="60" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G59" s="60" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H59" s="60" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I59" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J59" s="60" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="K59" s="55" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="L59"/>
       <c r="M59"/>
@@ -4892,25 +4874,25 @@
         <v>120</v>
       </c>
       <c r="E60" s="59" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F60" s="62" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G60" s="62" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="H60" s="62" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I60" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J60" s="62" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="K60" s="54" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="L60"/>
       <c r="M60"/>
@@ -4922,31 +4904,31 @@
         <v>52</v>
       </c>
       <c r="C61" s="65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="60" t="s">
         <v>121</v>
       </c>
       <c r="E61" s="60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F61" s="60" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G61" s="60" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H61" s="60" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="I61" s="60" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="J61" s="60" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="K61" s="55" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
       <c r="L61"/>
       <c r="M61"/>
@@ -4958,31 +4940,31 @@
         <v>53</v>
       </c>
       <c r="C62" s="64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D62" s="59" t="s">
         <v>122</v>
       </c>
       <c r="E62" s="59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F62" s="62" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G62" s="62" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H62" s="62" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I62" s="62" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="J62" s="62" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="K62" s="54" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="L62"/>
       <c r="M62"/>
@@ -4994,31 +4976,31 @@
         <v>54</v>
       </c>
       <c r="C63" s="65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D63" s="60" t="s">
         <v>123</v>
       </c>
       <c r="E63" s="60" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F63" s="60" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G63" s="60" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H63" s="60" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I63" s="60" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J63" s="60" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="K63" s="55" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L63"/>
       <c r="M63"/>
@@ -5036,25 +5018,25 @@
         <v>124</v>
       </c>
       <c r="E64" s="59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F64" s="62" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G64" s="62" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H64" s="62" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I64" s="62" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="J64" s="62" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="K64" s="54" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="L64"/>
       <c r="M64"/>
@@ -5072,25 +5054,25 @@
         <v>125</v>
       </c>
       <c r="E65" s="60" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F65" s="60" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G65" s="60" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H65" s="60" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I65" s="60" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="J65" s="60" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="K65" s="55" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="L65"/>
       <c r="M65"/>
@@ -5108,25 +5090,25 @@
         <v>126</v>
       </c>
       <c r="E66" s="59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F66" s="62" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G66" s="62" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H66" s="62" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I66" s="62" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="J66" s="62" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="K66" s="54" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="L66"/>
       <c r="M66"/>
@@ -5144,25 +5126,25 @@
         <v>127</v>
       </c>
       <c r="E67" s="60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F67" s="60" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G67" s="60" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H67" s="60" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="I67" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J67" s="60" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="K67" s="55" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="L67"/>
       <c r="M67"/>
@@ -5180,25 +5162,25 @@
         <v>128</v>
       </c>
       <c r="E68" s="59" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F68" s="62" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G68" s="62" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H68" s="62" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I68" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J68" s="62" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="K68" s="54" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="L68"/>
       <c r="M68"/>
@@ -5216,25 +5198,25 @@
         <v>129</v>
       </c>
       <c r="E69" s="60" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F69" s="60" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G69" s="60" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="H69" s="60" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="I69" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J69" s="60" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="K69" s="55" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="L69"/>
       <c r="M69"/>
@@ -5252,25 +5234,25 @@
         <v>130</v>
       </c>
       <c r="E70" s="59" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F70" s="62" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G70" s="62" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H70" s="62" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I70" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J70" s="62" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="K70" s="54" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="L70"/>
       <c r="M70"/>
@@ -5288,25 +5270,25 @@
         <v>131</v>
       </c>
       <c r="E71" s="60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F71" s="60" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G71" s="60" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H71" s="60" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I71" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J71" s="60" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="K71" s="55" t="s">
-        <v>523</v>
+        <v>392</v>
       </c>
       <c r="L71"/>
       <c r="M71"/>
@@ -5324,25 +5306,25 @@
         <v>132</v>
       </c>
       <c r="E72" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F72" s="62" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G72" s="62" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="H72" s="62" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I72" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J72" s="62" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="K72" s="54" t="s">
-        <v>396</v>
+        <v>515</v>
       </c>
       <c r="L72"/>
       <c r="M72"/>
@@ -5360,25 +5342,25 @@
         <v>133</v>
       </c>
       <c r="E73" s="60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F73" s="60" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G73" s="60" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="H73" s="60" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I73" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J73" s="60" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="K73" s="55" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="L73"/>
       <c r="M73"/>
@@ -5396,25 +5378,25 @@
         <v>134</v>
       </c>
       <c r="E74" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F74" s="62" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G74" s="62" t="s">
         <v>323</v>
       </c>
       <c r="H74" s="62" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I74" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J74" s="62" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="K74" s="54" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="L74"/>
       <c r="M74"/>
@@ -5432,25 +5414,25 @@
         <v>135</v>
       </c>
       <c r="E75" s="60" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F75" s="60" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G75" s="60" t="s">
         <v>326</v>
       </c>
       <c r="H75" s="60" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I75" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J75" s="60" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="K75" s="55" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="L75"/>
       <c r="M75"/>
@@ -5468,25 +5450,25 @@
         <v>136</v>
       </c>
       <c r="E76" s="59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F76" s="62" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G76" s="62" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H76" s="62" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I76" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J76" s="62" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="K76" s="54" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="L76"/>
       <c r="M76"/>
@@ -5504,25 +5486,25 @@
         <v>137</v>
       </c>
       <c r="E77" s="60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F77" s="60" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G77" s="60" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H77" s="60" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I77" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J77" s="60" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="K77" s="55" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="L77"/>
       <c r="M77"/>
@@ -5540,25 +5522,25 @@
         <v>138</v>
       </c>
       <c r="E78" s="59" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F78" s="62" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G78" s="62" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="H78" s="62" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I78" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J78" s="62" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="K78" s="54" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="L78"/>
       <c r="M78"/>
@@ -5576,25 +5558,25 @@
         <v>139</v>
       </c>
       <c r="E79" s="60" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F79" s="60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G79" s="60" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H79" s="60" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I79" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J79" s="60" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="K79" s="55" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="L79"/>
       <c r="M79"/>
@@ -5612,25 +5594,25 @@
         <v>140</v>
       </c>
       <c r="E80" s="59" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F80" s="62" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G80" s="62" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="H80" s="62" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I80" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J80" s="62" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="K80" s="54" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="L80"/>
       <c r="M80"/>
@@ -5648,25 +5630,25 @@
         <v>141</v>
       </c>
       <c r="E81" s="60" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F81" s="60" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G81" s="60" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="H81" s="60" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I81" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J81" s="60" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="K81" s="55" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="L81"/>
       <c r="M81"/>
@@ -5684,30 +5666,30 @@
         <v>142</v>
       </c>
       <c r="E82" s="59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F82" s="62" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G82" s="62" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H82" s="62" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I82" s="62" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J82" s="62" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="K82" s="54" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="L82"/>
       <c r="M82"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:12" s="3" customFormat="1" thickBot="1">
       <c r="A83" s="15"/>
       <c r="B83" s="58">
         <f>ROW(B83)-ROW($B$9)</f>
@@ -5720,85 +5702,64 @@
         <v>143</v>
       </c>
       <c r="E83" s="60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F83" s="60" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G83" s="60" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H83" s="60" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I83" s="60" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="J83" s="60" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="K83" s="55" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="L83"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="1:12" s="3" customFormat="1" thickBot="1">
+    <row r="84" spans="1:12">
       <c r="A84" s="15"/>
-      <c r="B84" s="57">
-        <f>ROW(B84)-ROW($B$9)</f>
-        <v>75</v>
-      </c>
-      <c r="C84" s="64">
-        <v>1</v>
-      </c>
-      <c r="D84" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="E84" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="F84" s="62" t="s">
-        <v>295</v>
-      </c>
-      <c r="G84" s="62" t="s">
-        <v>332</v>
-      </c>
-      <c r="H84" s="62" t="s">
-        <v>408</v>
-      </c>
-      <c r="I84" s="62" t="s">
-        <v>410</v>
-      </c>
-      <c r="J84" s="62" t="s">
-        <v>487</v>
-      </c>
-      <c r="K84" s="54" t="s">
-        <v>531</v>
+      <c r="B84" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="C84" s="73"/>
+      <c r="D84" s="73"/>
+      <c r="E84" s="52"/>
+      <c r="F84" s="51"/>
+      <c r="G84" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H84"/>
+      <c r="I84"/>
+      <c r="J84" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="K84" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="L84"/>
       <c r="M84"/>
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="15"/>
-      <c r="B85" s="72" t="s">
-        <v>35</v>
-      </c>
-      <c r="C85" s="73"/>
-      <c r="D85" s="73"/>
-      <c r="E85" s="52"/>
-      <c r="F85" s="51"/>
-      <c r="G85" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H85"/>
-      <c r="I85"/>
-      <c r="J85" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="K85" s="53" t="s">
-        <v>67</v>
-      </c>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="20"/>
       <c r="L85"/>
       <c r="M85"/>
     </row>
@@ -5807,13 +5768,13 @@
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
-      <c r="J86" s="9"/>
-      <c r="K86" s="20"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="10"/>
+      <c r="K86" s="21"/>
       <c r="L86"/>
       <c r="M86"/>
     </row>
@@ -5827,42 +5788,34 @@
       <c r="G87" s="10"/>
       <c r="H87" s="10"/>
       <c r="I87" s="10"/>
-      <c r="J87" s="10"/>
+      <c r="J87" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="K87" s="21"/>
       <c r="L87"/>
       <c r="M87"/>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:11" thickBot="1">
       <c r="A88" s="15"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="10"/>
-      <c r="J88" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K88" s="21"/>
+      <c r="B88" s="49"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
+      <c r="J88" s="17"/>
+      <c r="K88" s="22"/>
       <c r="L88"/>
       <c r="M88"/>
     </row>
-    <row r="89" spans="1:11" thickBot="1">
-      <c r="A89" s="15"/>
-      <c r="B89" s="49"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="22"/>
-      <c r="L89"/>
-      <c r="M89"/>
+    <row r="90" spans="1:11">
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90"/>
+      <c r="H90"/>
     </row>
     <row r="91" spans="1:11">
       <c r="D91" s="1"/>
@@ -5878,16 +5831,9 @@
       <c r="G92"/>
       <c r="H92"/>
     </row>
-    <row r="93" spans="1:11">
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93"/>
-      <c r="H93"/>
-    </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B84:D84"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.46" right="0.36" top="0.58" bottom="1" header="0.5" footer="0.5"/>
@@ -5917,7 +5863,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -5957,7 +5903,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -5967,7 +5913,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -6007,7 +5953,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -6017,7 +5963,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6027,7 +5973,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -6037,7 +5983,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -6047,7 +5993,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -6057,7 +6003,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -6067,7 +6013,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>

</xml_diff>